<commit_message>
Adding a style file Modifing radio button to click on text.
</commit_message>
<xml_diff>
--- a/Coop.xlsx
+++ b/Coop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samis-mac/My Drive/Courses/Fullstack-Development/Palletize-JS/client-only/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samis-mac/My Drive/Courses/Fullstack-Development/Palletize-JS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9357708A-0E21-0740-BC0B-618932FB69A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20C6FCD-9869-1948-9F91-D38A608E8B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33240" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{176E6E39-73AA-8C43-80B7-FB166E0FB9CC}"/>
+    <workbookView xWindow="8180" yWindow="2320" windowWidth="28040" windowHeight="17440" xr2:uid="{176E6E39-73AA-8C43-80B7-FB166E0FB9CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -434,7 +433,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>